<commit_message>
Revenue Security Division - SE Federal Tax Statistics
</commit_message>
<xml_diff>
--- a/DES/LSD/LSD.REFERENCE.xlsx
+++ b/DES/LSD/LSD.REFERENCE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LSD.REFERENCE" sheetId="1" state="visible" r:id="rId3"/>
@@ -2796,7 +2796,7 @@
   </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -2948,7 +2948,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="C10 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3065,7 +3065,7 @@
   <dimension ref="A1:F164"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C10 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5796,8 +5796,8 @@
   </sheetPr>
   <dimension ref="A1:E166"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="1" sqref="C10 B29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>